<commit_message>
Working on performance section
</commit_message>
<xml_diff>
--- a/results/ParallelSort.xlsx
+++ b/results/ParallelSort.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jj.lay\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jj.lay\source\github\COMS7900ParallelSort\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707ED072-1A14-4970-8EDC-AC8810C2E497}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA689F5B-FE0C-444F-8929-68056FF3BF58}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B3FED0E2-B4B8-4D46-8D42-356631E4E73A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{B3FED0E2-B4B8-4D46-8D42-356631E4E73A}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -429,6 +429,9 @@
       <c:pivotFmt>
         <c:idx val="7"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="38100" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -456,6 +459,9 @@
       <c:pivotFmt>
         <c:idx val="8"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="38100" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -483,6 +489,9 @@
       <c:pivotFmt>
         <c:idx val="9"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="38100" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -537,6 +546,9 @@
       <c:pivotFmt>
         <c:idx val="11"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="38100" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -564,6 +576,9 @@
       <c:pivotFmt>
         <c:idx val="12"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="38100" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -591,6 +606,9 @@
       <c:pivotFmt>
         <c:idx val="13"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="38100" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -4865,7 +4883,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0F5DF196-3479-4BAE-95BB-F06F3139F992}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4972,7 +4990,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670192" cy="6293013"/>
+    <xdr:ext cx="8661400" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5121,7 +5139,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670192" cy="6293013"/>
+    <xdr:ext cx="8662051" cy="6293013"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5611,7 +5629,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EE72D345-56C7-4C85-9011-32024D05021A}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EE72D345-56C7-4C85-9011-32024D05021A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A3:C11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -6201,8 +6219,8 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6953,10 +6971,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5659036E-20D9-468A-9C58-98BCDD0F4257}">
-  <dimension ref="A2:J8"/>
+  <dimension ref="A2:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6970,10 +6988,10 @@
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -7004,8 +7022,12 @@
       <c r="J2" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="M2" t="str">
+        <f>A2&amp; " &amp; " &amp;B2&amp; " &amp; " &amp;C2&amp; " &amp; " &amp;D2&amp; " &amp; " &amp;E2&amp; " &amp; " &amp;F2&amp; " &amp; " &amp;G2&amp; " &amp; " &amp;H2&amp; " &amp; " &amp;I2&amp; " &amp; " &amp;J2&amp;" \\"</f>
+        <v>Nodes &amp; initializeMPI &amp; distributeFileNames &amp; importData &amp; sortData &amp; exchangeMinMax &amp; adaptBins &amp; swapData &amp; sortData &amp; Total \\</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>256</v>
       </c>
@@ -7034,11 +7056,15 @@
         <v>0.03</v>
       </c>
       <c r="J3" s="3">
-        <f>SUM(B3:I3)</f>
+        <f t="shared" ref="J3:J8" si="0">SUM(B3:I3)</f>
         <v>282.96999999999997</v>
       </c>
+      <c r="M3" t="str">
+        <f>A3&amp; " &amp; " &amp;B3&amp; " &amp; " &amp;C3&amp; " &amp; " &amp;D3&amp; " &amp; " &amp;E3&amp; " &amp; " &amp;F3&amp; " &amp; " &amp;G3&amp; " &amp; " &amp;H3&amp; " &amp; " &amp;I3&amp; " &amp; " &amp;J3&amp;" \\"</f>
+        <v>256 &amp; 0 &amp; 0.25 &amp; 0.95 &amp; 0.03 &amp; 0 &amp; 44.96 &amp; 236.75 &amp; 0.03 &amp; 282.97 \\</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>128</v>
       </c>
@@ -7067,11 +7093,15 @@
         <v>0.12</v>
       </c>
       <c r="J4" s="3">
-        <f>SUM(B4:I4)</f>
+        <f t="shared" si="0"/>
         <v>137.73999999999998</v>
       </c>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M8" si="1">A4&amp; " &amp; " &amp;B4&amp; " &amp; " &amp;C4&amp; " &amp; " &amp;D4&amp; " &amp; " &amp;E4&amp; " &amp; " &amp;F4&amp; " &amp; " &amp;G4&amp; " &amp; " &amp;H4&amp; " &amp; " &amp;I4&amp; " &amp; " &amp;J4&amp;" \\"</f>
+        <v>128 &amp; 0 &amp; 0.16 &amp; 0.03 &amp; 0.12 &amp; 0 &amp; 6.08 &amp; 131.23 &amp; 0.12 &amp; 137.74 \\</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>64</v>
       </c>
@@ -7100,11 +7130,15 @@
         <v>0.35</v>
       </c>
       <c r="J5" s="3">
-        <f>SUM(B5:I5)</f>
+        <f t="shared" si="0"/>
         <v>68.27</v>
       </c>
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>64 &amp; 0 &amp; 0.13 &amp; 2.74 &amp; 0.35 &amp; 0 &amp; 0.72 &amp; 63.98 &amp; 0.35 &amp; 68.27 \\</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>32</v>
       </c>
@@ -7133,11 +7167,15 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="J6" s="3">
-        <f>SUM(B6:I6)</f>
+        <f t="shared" si="0"/>
         <v>40.779999999999994</v>
       </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>32 &amp; 0 &amp; 0.05 &amp; 2.42 &amp; 1.12 &amp; 0 &amp; 4.81 &amp; 31.26 &amp; 1.12 &amp; 40.78 \\</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16</v>
       </c>
@@ -7166,11 +7204,15 @@
         <v>6.46</v>
       </c>
       <c r="J7" s="3">
-        <f>SUM(B7:I7)</f>
+        <f t="shared" si="0"/>
         <v>30.75</v>
       </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>16 &amp; 0 &amp; 0.1 &amp; 2.66 &amp; 6.46 &amp; 0 &amp; 0.02 &amp; 15.05 &amp; 6.46 &amp; 30.75 \\</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -7199,8 +7241,12 @@
         <v>39.61</v>
       </c>
       <c r="J8" s="3">
-        <f>SUM(B8:I8)</f>
+        <f t="shared" si="0"/>
         <v>89.28</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>8 &amp; 0 &amp; 0.02 &amp; 3.03 &amp; 39.61 &amp; 0 &amp; 0.01 &amp; 7 &amp; 39.61 &amp; 89.28 \\</v>
       </c>
     </row>
   </sheetData>

</xml_diff>